<commit_message>
Versión 210413 - final
</commit_message>
<xml_diff>
--- a/TFC - Textos/Plantilla-resultados-final.xlsx
+++ b/TFC - Textos/Plantilla-resultados-final.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23117"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500" firstSheet="7" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Páginas de inicio" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="962" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="308">
   <si>
     <t>PÁGINAS DE INICIO</t>
   </si>
@@ -1179,6 +1179,12 @@
   </si>
   <si>
     <t>El usuario puede disfrutar de todos los contenidos sin necesidad de tener que instalar plugins adicionales</t>
+  </si>
+  <si>
+    <t>Puntuación</t>
+  </si>
+  <si>
+    <t>Ciudad</t>
   </si>
 </sst>
 </file>
@@ -1258,7 +1264,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1280,6 +1286,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1402,7 +1414,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="29">
+  <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1432,8 +1444,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1593,6 +1607,48 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1611,6 +1667,45 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1620,21 +1715,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1644,74 +1724,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="29">
+  <cellStyles count="31">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
@@ -1726,6 +1743,7 @@
     <cellStyle name="Hipervínculo" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
@@ -1740,6 +1758,7 @@
     <cellStyle name="Hipervínculo visitado" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2077,8 +2096,8 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
+      <pane ySplit="2" topLeftCell="A16" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" sqref="A1:D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2086,7 +2105,7 @@
     <col min="1" max="1" width="41.83203125" style="48" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="9.33203125" style="48" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="48" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" style="92" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" style="67" customWidth="1"/>
     <col min="6" max="6" width="6.6640625" style="48" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.83203125" style="48" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.5" style="48" bestFit="1" customWidth="1"/>
@@ -2096,14 +2115,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="88"/>
-      <c r="F1" s="46" t="s">
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="94" t="s">
         <v>8</v>
       </c>
       <c r="G1" s="43" t="s">
@@ -2130,7 +2149,7 @@
       <c r="D2" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="89"/>
+      <c r="E2" s="64"/>
       <c r="F2" s="46"/>
       <c r="G2" s="39" t="s">
         <v>10</v>
@@ -2149,10 +2168,10 @@
       <c r="A3" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="59"/>
-      <c r="C3" s="59"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="89"/>
+      <c r="B3" s="73"/>
+      <c r="C3" s="73"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="64"/>
       <c r="F3" s="51"/>
       <c r="G3" s="41"/>
       <c r="H3" s="52"/>
@@ -2172,7 +2191,7 @@
       <c r="D4" s="43" t="s">
         <v>292</v>
       </c>
-      <c r="E4" s="90">
+      <c r="E4" s="65">
         <f>SUM((IF(B4="Sí",3,IF(B4="Regular",2,IF(B4="Parcialmente",2)))),(IF(C4="Sí",3,IF(C4="Regular",2,IF(C4="Parcialmente",2)))),(IF(D4="Sí",3,IF(D4="Regular",2,IF(D4="Parcialmente",2)))))/9</f>
         <v>1</v>
       </c>
@@ -2185,10 +2204,10 @@
       <c r="A5" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="55"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="57"/>
-      <c r="E5" s="90">
+      <c r="B5" s="69"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="65">
         <f t="shared" ref="E5:E22" si="0">SUM((IF(B5="Sí",3,IF(B5="Regular",2,IF(B5="Parcialmente",2)))),(IF(C5="Sí",3,IF(C5="Regular",2,IF(C5="Parcialmente",2)))),(IF(D5="Sí",3,IF(D5="Regular",2,IF(D5="Parcialmente",2)))))/9</f>
         <v>0</v>
       </c>
@@ -2208,7 +2227,7 @@
       <c r="D6" s="43" t="s">
         <v>292</v>
       </c>
-      <c r="E6" s="90">
+      <c r="E6" s="65">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
@@ -2227,7 +2246,7 @@
       <c r="D7" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="90">
+      <c r="E7" s="65">
         <f t="shared" si="0"/>
         <v>0.55555555555555558</v>
       </c>
@@ -2246,7 +2265,7 @@
       <c r="D8" s="43" t="s">
         <v>292</v>
       </c>
-      <c r="E8" s="90">
+      <c r="E8" s="65">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -2269,7 +2288,7 @@
       <c r="D9" s="43" t="s">
         <v>292</v>
       </c>
-      <c r="E9" s="90">
+      <c r="E9" s="65">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -2279,10 +2298,10 @@
       <c r="A10" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="55"/>
-      <c r="C10" s="56"/>
-      <c r="D10" s="57"/>
-      <c r="E10" s="90">
+      <c r="B10" s="69"/>
+      <c r="C10" s="70"/>
+      <c r="D10" s="71"/>
+      <c r="E10" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2301,7 +2320,7 @@
       <c r="D11" s="43" t="s">
         <v>292</v>
       </c>
-      <c r="E11" s="90">
+      <c r="E11" s="65">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -2320,7 +2339,7 @@
       <c r="D12" s="43" t="s">
         <v>293</v>
       </c>
-      <c r="E12" s="90">
+      <c r="E12" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2339,7 +2358,7 @@
       <c r="D13" s="43" t="s">
         <v>293</v>
       </c>
-      <c r="E13" s="90">
+      <c r="E13" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2358,7 +2377,7 @@
       <c r="D14" s="43" t="s">
         <v>293</v>
       </c>
-      <c r="E14" s="90">
+      <c r="E14" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2377,7 +2396,7 @@
       <c r="D15" s="43" t="s">
         <v>294</v>
       </c>
-      <c r="E15" s="90">
+      <c r="E15" s="65">
         <f>SUM((IF(B15="Sí",3,IF(B15="Regular",2,IF(B15="Parcialmente",2,IF(B15="Extra",3))))),(IF(C15="Sí",3,IF(C15="Regular",2,IF(C15="Parcialmente",2,IF(C15="Extra",3))))),(IF(D15="Sí",3,IF(D15="Regular",2,IF(D15="Parcialmente",2,IF(D15="Extra",3))))))/9</f>
         <v>1</v>
       </c>
@@ -2390,10 +2409,10 @@
       <c r="A16" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="55"/>
-      <c r="C16" s="56"/>
-      <c r="D16" s="57"/>
-      <c r="E16" s="90"/>
+      <c r="B16" s="69"/>
+      <c r="C16" s="70"/>
+      <c r="D16" s="71"/>
+      <c r="E16" s="65"/>
       <c r="F16" s="53"/>
     </row>
     <row r="17" spans="1:6">
@@ -2409,7 +2428,7 @@
       <c r="D17" s="43" t="s">
         <v>292</v>
       </c>
-      <c r="E17" s="90">
+      <c r="E17" s="65">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -2428,7 +2447,7 @@
       <c r="D18" s="43" t="s">
         <v>293</v>
       </c>
-      <c r="E18" s="90">
+      <c r="E18" s="65">
         <f t="shared" si="0"/>
         <v>0.66666666666666663</v>
       </c>
@@ -2447,7 +2466,7 @@
       <c r="D19" s="43" t="s">
         <v>293</v>
       </c>
-      <c r="E19" s="90">
+      <c r="E19" s="65">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
@@ -2466,7 +2485,7 @@
       <c r="D20" s="43" t="s">
         <v>292</v>
       </c>
-      <c r="E20" s="90">
+      <c r="E20" s="65">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
@@ -2485,7 +2504,7 @@
       <c r="D21" s="43" t="s">
         <v>293</v>
       </c>
-      <c r="E21" s="90">
+      <c r="E21" s="65">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
@@ -2504,7 +2523,7 @@
       <c r="D22" s="43" t="s">
         <v>292</v>
       </c>
-      <c r="E22" s="90">
+      <c r="E22" s="65">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -2512,33 +2531,55 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="54"/>
-      <c r="B23" s="54"/>
-      <c r="C23" s="54"/>
-      <c r="D23" s="54"/>
-      <c r="E23" s="91"/>
+      <c r="B23" s="54">
+        <v>23</v>
+      </c>
+      <c r="C23" s="54">
+        <v>17</v>
+      </c>
+      <c r="D23" s="54">
+        <v>20</v>
+      </c>
+      <c r="E23" s="66"/>
       <c r="F23" s="53"/>
     </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="54"/>
-      <c r="B24" s="54"/>
+    <row r="24" spans="1:6" ht="24">
+      <c r="A24" s="42" t="s">
+        <v>307</v>
+      </c>
+      <c r="B24" s="42" t="s">
+        <v>306</v>
+      </c>
       <c r="C24" s="54"/>
       <c r="D24" s="54"/>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="54"/>
-      <c r="B25" s="54"/>
+      <c r="A25" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" s="42">
+        <v>23</v>
+      </c>
       <c r="C25" s="54"/>
       <c r="D25" s="54"/>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="54"/>
-      <c r="B26" s="54"/>
+      <c r="A26" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="42">
+        <v>17</v>
+      </c>
       <c r="C26" s="54"/>
       <c r="D26" s="54"/>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="54"/>
-      <c r="B27" s="54"/>
+      <c r="A27" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" s="42">
+        <v>20</v>
+      </c>
       <c r="C27" s="54"/>
       <c r="D27" s="54"/>
     </row>
@@ -2608,7 +2649,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
@@ -2620,12 +2661,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="83" t="s">
         <v>216</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="66"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="85"/>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5" ht="16" thickBot="1">
@@ -2645,9 +2686,9 @@
       <c r="A3" s="14" t="s">
         <v>217</v>
       </c>
-      <c r="B3" s="67"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="68"/>
+      <c r="B3" s="86"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="87"/>
       <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:5">
@@ -2834,9 +2875,9 @@
       <c r="A16" s="13" t="s">
         <v>230</v>
       </c>
-      <c r="B16" s="61"/>
-      <c r="C16" s="62"/>
-      <c r="D16" s="63"/>
+      <c r="B16" s="88"/>
+      <c r="C16" s="89"/>
+      <c r="D16" s="90"/>
       <c r="E16" s="8"/>
     </row>
     <row r="17" spans="1:5">
@@ -2970,7 +3011,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
@@ -2982,12 +3023,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18" customHeight="1">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="83" t="s">
         <v>239</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="66"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="85"/>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:6" ht="16" thickBot="1">
@@ -3007,9 +3048,9 @@
       <c r="A3" s="14" t="s">
         <v>240</v>
       </c>
-      <c r="B3" s="67"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="68"/>
+      <c r="B3" s="86"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="87"/>
       <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:6">
@@ -3061,9 +3102,9 @@
       <c r="A7" s="13" t="s">
         <v>244</v>
       </c>
-      <c r="B7" s="61"/>
-      <c r="C7" s="62"/>
-      <c r="D7" s="63"/>
+      <c r="B7" s="88"/>
+      <c r="C7" s="89"/>
+      <c r="D7" s="90"/>
       <c r="E7" s="8"/>
     </row>
     <row r="8" spans="1:6">
@@ -3166,9 +3207,9 @@
       <c r="A15" s="13" t="s">
         <v>252</v>
       </c>
-      <c r="B15" s="61"/>
-      <c r="C15" s="62"/>
-      <c r="D15" s="63"/>
+      <c r="B15" s="88"/>
+      <c r="C15" s="89"/>
+      <c r="D15" s="90"/>
     </row>
     <row r="16" spans="1:6" ht="30">
       <c r="A16" s="4" t="s">
@@ -3247,9 +3288,9 @@
       <c r="A21" s="13" t="s">
         <v>258</v>
       </c>
-      <c r="B21" s="61"/>
-      <c r="C21" s="62"/>
-      <c r="D21" s="63"/>
+      <c r="B21" s="88"/>
+      <c r="C21" s="89"/>
+      <c r="D21" s="90"/>
     </row>
     <row r="22" spans="1:4" ht="45">
       <c r="A22" s="4" t="s">
@@ -3283,9 +3324,9 @@
       <c r="A24" s="13" t="s">
         <v>261</v>
       </c>
-      <c r="B24" s="61"/>
-      <c r="C24" s="62"/>
-      <c r="D24" s="63"/>
+      <c r="B24" s="88"/>
+      <c r="C24" s="89"/>
+      <c r="D24" s="90"/>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="4" t="s">
@@ -3339,30 +3380,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A4" activePane="bottomLeft" state="frozenSplit"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="37" style="48" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" style="74" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" style="74" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" style="74" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" style="57" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" style="57" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" style="57" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2" style="48" customWidth="1"/>
-    <col min="6" max="6" width="9" style="78" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" style="58" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" style="48" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="10.83203125" style="48"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="17" customHeight="1">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="78" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="77"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="80"/>
       <c r="E1" s="45"/>
     </row>
     <row r="2" spans="1:9" ht="13" thickBot="1">
@@ -3382,9 +3423,9 @@
       <c r="A3" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="79"/>
-      <c r="C3" s="79"/>
-      <c r="D3" s="80"/>
+      <c r="B3" s="81"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="82"/>
       <c r="E3" s="51"/>
     </row>
     <row r="4" spans="1:9">
@@ -3401,13 +3442,13 @@
         <v>292</v>
       </c>
       <c r="E4" s="52"/>
-      <c r="F4" s="78">
+      <c r="F4" s="58">
         <f>SUM((IF(B4="Sí",3,IF(B4="Regular",2))),(IF(C4="Sí",3,IF(C4="Regular",2))),(IF(D4="Sí",3,IF(D4="Regular",2))))/9</f>
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="72" t="s">
+      <c r="A5" s="55" t="s">
         <v>37</v>
       </c>
       <c r="B5" s="43" t="s">
@@ -3420,7 +3461,7 @@
         <v>18</v>
       </c>
       <c r="E5" s="53"/>
-      <c r="F5" s="78">
+      <c r="F5" s="58">
         <f>SUM((IF(B5="Sí",3,IF(B5="Regular",2,IF(B5="Parcialmente",2)))),(IF(C5="Sí",3,IF(C5="Regular",2,IF(C5="Parcialmente",2)))),(IF(D5="Sí",3,IF(D5="Regular",2,IF(D5="Parcialmente",2)))))/9</f>
         <v>0.88888888888888884</v>
       </c>
@@ -3439,8 +3480,8 @@
         <v>145</v>
       </c>
       <c r="E6" s="53"/>
-      <c r="F6" s="78">
-        <f t="shared" ref="F4:F8" si="0">SUM((IF(B6="Sí",3,IF(B6="Regular",2))),(IF(C6="Sí",3,IF(C6="Regular",2))),(IF(D6="Sí",3,IF(D6="Regular",2))))/9</f>
+      <c r="F6" s="58">
+        <f t="shared" ref="F6:F8" si="0">SUM((IF(B6="Sí",3,IF(B6="Regular",2))),(IF(C6="Sí",3,IF(C6="Regular",2))),(IF(D6="Sí",3,IF(D6="Regular",2))))/9</f>
         <v>0.77777777777777779</v>
       </c>
     </row>
@@ -3458,7 +3499,7 @@
         <v>292</v>
       </c>
       <c r="E7" s="53"/>
-      <c r="F7" s="78">
+      <c r="F7" s="58">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -3477,7 +3518,7 @@
         <v>292</v>
       </c>
       <c r="E8" s="53"/>
-      <c r="F8" s="78">
+      <c r="F8" s="58">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -3503,7 +3544,7 @@
         <v>145</v>
       </c>
       <c r="E9" s="53"/>
-      <c r="F9" s="78">
+      <c r="F9" s="58">
         <f>SUM((IF(B9="Sí",3,IF(B9="Regular",2))),(IF(C9="Sí",3,IF(C9="Regular",2))),(IF(D9="Sí",3,IF(D9="Regular",2))))/9</f>
         <v>0.88888888888888884</v>
       </c>
@@ -3512,7 +3553,7 @@
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="72" t="s">
+      <c r="A10" s="55" t="s">
         <v>42</v>
       </c>
       <c r="B10" s="43" t="s">
@@ -3525,7 +3566,7 @@
         <v>145</v>
       </c>
       <c r="E10" s="53"/>
-      <c r="F10" s="78">
+      <c r="F10" s="58">
         <f t="shared" ref="F10:F49" si="1">SUM((IF(B10="Sí",3,IF(B10="Regular",2))),(IF(C10="Sí",3,IF(C10="Regular",2))),(IF(D10="Sí",3,IF(D10="Regular",2))))/9</f>
         <v>0.88888888888888884</v>
       </c>
@@ -3547,7 +3588,7 @@
         <v>293</v>
       </c>
       <c r="E11" s="53"/>
-      <c r="F11" s="78">
+      <c r="F11" s="58">
         <f t="shared" si="1"/>
         <v>0.22222222222222221</v>
       </c>
@@ -3566,7 +3607,7 @@
         <v>293</v>
       </c>
       <c r="E12" s="53"/>
-      <c r="F12" s="78">
+      <c r="F12" s="58">
         <f t="shared" si="1"/>
         <v>0.55555555555555558</v>
       </c>
@@ -3585,7 +3626,7 @@
         <v>145</v>
       </c>
       <c r="E13" s="53"/>
-      <c r="F13" s="78">
+      <c r="F13" s="58">
         <f t="shared" si="1"/>
         <v>0.88888888888888884</v>
       </c>
@@ -3594,9 +3635,9 @@
       <c r="A14" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="81"/>
-      <c r="C14" s="82"/>
-      <c r="D14" s="83"/>
+      <c r="B14" s="75"/>
+      <c r="C14" s="76"/>
+      <c r="D14" s="77"/>
       <c r="E14" s="53"/>
     </row>
     <row r="15" spans="1:9">
@@ -3613,7 +3654,7 @@
         <v>292</v>
       </c>
       <c r="E15" s="53"/>
-      <c r="F15" s="78">
+      <c r="F15" s="58">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -3632,7 +3673,7 @@
         <v>292</v>
       </c>
       <c r="E16" s="53"/>
-      <c r="F16" s="78">
+      <c r="F16" s="58">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -3651,7 +3692,7 @@
         <v>145</v>
       </c>
       <c r="E17" s="53"/>
-      <c r="F17" s="78">
+      <c r="F17" s="58">
         <f t="shared" si="1"/>
         <v>0.66666666666666663</v>
       </c>
@@ -3670,7 +3711,7 @@
         <v>145</v>
       </c>
       <c r="E18" s="53"/>
-      <c r="F18" s="78">
+      <c r="F18" s="58">
         <f t="shared" si="1"/>
         <v>0.66666666666666663</v>
       </c>
@@ -3689,7 +3730,7 @@
         <v>293</v>
       </c>
       <c r="E19" s="53"/>
-      <c r="F19" s="78">
+      <c r="F19" s="58">
         <f t="shared" si="1"/>
         <v>0.55555555555555558</v>
       </c>
@@ -3708,7 +3749,7 @@
         <v>292</v>
       </c>
       <c r="E20" s="53"/>
-      <c r="F20" s="78">
+      <c r="F20" s="58">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -3717,9 +3758,9 @@
       <c r="A21" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="84"/>
-      <c r="C21" s="85"/>
-      <c r="D21" s="86"/>
+      <c r="B21" s="59"/>
+      <c r="C21" s="60"/>
+      <c r="D21" s="61"/>
       <c r="E21" s="53"/>
     </row>
     <row r="22" spans="1:6">
@@ -3735,7 +3776,7 @@
       <c r="D22" s="43" t="s">
         <v>292</v>
       </c>
-      <c r="F22" s="78">
+      <c r="F22" s="58">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -3753,7 +3794,7 @@
       <c r="D23" s="43" t="s">
         <v>292</v>
       </c>
-      <c r="F23" s="78">
+      <c r="F23" s="58">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -3771,7 +3812,7 @@
       <c r="D24" s="43" t="s">
         <v>292</v>
       </c>
-      <c r="F24" s="78">
+      <c r="F24" s="58">
         <f t="shared" si="1"/>
         <v>0.66666666666666663</v>
       </c>
@@ -3789,7 +3830,7 @@
       <c r="D25" s="43" t="s">
         <v>293</v>
       </c>
-      <c r="F25" s="78">
+      <c r="F25" s="58">
         <f t="shared" si="1"/>
         <v>0.66666666666666663</v>
       </c>
@@ -3807,7 +3848,7 @@
       <c r="D26" s="43" t="s">
         <v>292</v>
       </c>
-      <c r="F26" s="78">
+      <c r="F26" s="58">
         <f t="shared" si="1"/>
         <v>0.66666666666666663</v>
       </c>
@@ -3816,9 +3857,9 @@
       <c r="A27" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="B27" s="81"/>
-      <c r="C27" s="82"/>
-      <c r="D27" s="83"/>
+      <c r="B27" s="75"/>
+      <c r="C27" s="76"/>
+      <c r="D27" s="77"/>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="42" t="s">
@@ -3833,7 +3874,7 @@
       <c r="D28" s="43" t="s">
         <v>293</v>
       </c>
-      <c r="F28" s="78">
+      <c r="F28" s="58">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3851,7 +3892,7 @@
       <c r="D29" s="43" t="s">
         <v>293</v>
       </c>
-      <c r="F29" s="78">
+      <c r="F29" s="58">
         <f t="shared" si="1"/>
         <v>0.66666666666666663</v>
       </c>
@@ -3869,7 +3910,7 @@
       <c r="D30" s="43" t="s">
         <v>292</v>
       </c>
-      <c r="F30" s="78">
+      <c r="F30" s="58">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -3887,7 +3928,7 @@
       <c r="D31" s="43" t="s">
         <v>293</v>
       </c>
-      <c r="F31" s="78">
+      <c r="F31" s="58">
         <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
@@ -3905,7 +3946,7 @@
       <c r="D32" s="43" t="s">
         <v>293</v>
       </c>
-      <c r="F32" s="78">
+      <c r="F32" s="58">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3923,7 +3964,7 @@
       <c r="D33" s="43" t="s">
         <v>293</v>
       </c>
-      <c r="F33" s="78">
+      <c r="F33" s="58">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3941,7 +3982,7 @@
       <c r="D34" s="43" t="s">
         <v>292</v>
       </c>
-      <c r="F34" s="78">
+      <c r="F34" s="58">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -3959,7 +4000,7 @@
       <c r="D35" s="43" t="s">
         <v>293</v>
       </c>
-      <c r="F35" s="78">
+      <c r="F35" s="58">
         <f t="shared" si="1"/>
         <v>0.66666666666666663</v>
       </c>
@@ -3977,7 +4018,7 @@
       <c r="D36" s="43" t="s">
         <v>293</v>
       </c>
-      <c r="F36" s="78">
+      <c r="F36" s="58">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3995,7 +4036,7 @@
       <c r="D37" s="43" t="s">
         <v>293</v>
       </c>
-      <c r="F37" s="78">
+      <c r="F37" s="58">
         <f t="shared" si="1"/>
         <v>0.66666666666666663</v>
       </c>
@@ -4013,7 +4054,7 @@
       <c r="D38" s="43" t="s">
         <v>293</v>
       </c>
-      <c r="F38" s="78">
+      <c r="F38" s="58">
         <f t="shared" si="1"/>
         <v>0.66666666666666663</v>
       </c>
@@ -4031,7 +4072,7 @@
       <c r="D39" s="43" t="s">
         <v>292</v>
       </c>
-      <c r="F39" s="78">
+      <c r="F39" s="58">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -4049,7 +4090,7 @@
       <c r="D40" s="43" t="s">
         <v>293</v>
       </c>
-      <c r="F40" s="78">
+      <c r="F40" s="58">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4067,7 +4108,7 @@
       <c r="D41" s="43" t="s">
         <v>292</v>
       </c>
-      <c r="F41" s="78">
+      <c r="F41" s="58">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -4085,7 +4126,7 @@
       <c r="D42" s="43" t="s">
         <v>293</v>
       </c>
-      <c r="F42" s="78">
+      <c r="F42" s="58">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4103,7 +4144,7 @@
       <c r="D43" s="43" t="s">
         <v>292</v>
       </c>
-      <c r="F43" s="78">
+      <c r="F43" s="58">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -4121,7 +4162,7 @@
       <c r="D44" s="43" t="s">
         <v>293</v>
       </c>
-      <c r="F44" s="78">
+      <c r="F44" s="58">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4139,7 +4180,7 @@
       <c r="D45" s="43" t="s">
         <v>292</v>
       </c>
-      <c r="F45" s="78">
+      <c r="F45" s="58">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -4157,7 +4198,7 @@
       <c r="D46" s="43" t="s">
         <v>293</v>
       </c>
-      <c r="F46" s="78">
+      <c r="F46" s="58">
         <f t="shared" si="1"/>
         <v>0.66666666666666663</v>
       </c>
@@ -4175,25 +4216,25 @@
       <c r="D47" s="43" t="s">
         <v>293</v>
       </c>
-      <c r="F47" s="78">
+      <c r="F47" s="58">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="24">
-      <c r="A48" s="73" t="s">
+      <c r="A48" s="56" t="s">
         <v>297</v>
       </c>
-      <c r="B48" s="87" t="s">
+      <c r="B48" s="62" t="s">
         <v>289</v>
       </c>
-      <c r="C48" s="87" t="s">
+      <c r="C48" s="62" t="s">
         <v>290</v>
       </c>
-      <c r="D48" s="87" t="s">
+      <c r="D48" s="62" t="s">
         <v>291</v>
       </c>
-      <c r="F48" s="78">
+      <c r="F48" s="58">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4211,13 +4252,13 @@
       <c r="D49" s="43" t="s">
         <v>293</v>
       </c>
-      <c r="F49" s="78">
+      <c r="F49" s="58">
         <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="24">
-      <c r="B50" s="74" t="s">
+      <c r="B50" s="57" t="s">
         <v>295</v>
       </c>
     </row>
@@ -4253,18 +4294,18 @@
     <col min="1" max="1" width="36" style="48" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="11" style="48" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2" style="48" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" style="92" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" style="67" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="2.5" style="48" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="10.83203125" style="48"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="78" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="77"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="80"/>
       <c r="E1" s="45"/>
     </row>
     <row r="2" spans="1:7" ht="13" thickBot="1">
@@ -4284,9 +4325,9 @@
       <c r="A3" s="40" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="79"/>
-      <c r="C3" s="79"/>
-      <c r="D3" s="80"/>
+      <c r="B3" s="81"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="82"/>
       <c r="E3" s="51"/>
     </row>
     <row r="4" spans="1:7">
@@ -4303,13 +4344,13 @@
         <v>292</v>
       </c>
       <c r="E4" s="52"/>
-      <c r="F4" s="92">
-        <f t="shared" ref="F4:F7" si="0">SUM((IF(B4="Sí",3,IF(B4="Regular",2,IF(B4="Parcialmente",2)))),(IF(C4="Sí",3,IF(C4="Regular",2,IF(C4="Parcialmente",2)))),(IF(D4="Sí",3,IF(D4="Regular",2,IF(D4="Parcialmente",2)))))/9</f>
+      <c r="F4" s="67">
+        <f t="shared" ref="F4:F6" si="0">SUM((IF(B4="Sí",3,IF(B4="Regular",2,IF(B4="Parcialmente",2)))),(IF(C4="Sí",3,IF(C4="Regular",2,IF(C4="Parcialmente",2)))),(IF(D4="Sí",3,IF(D4="Regular",2,IF(D4="Parcialmente",2)))))/9</f>
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="72" t="s">
+      <c r="A5" s="55" t="s">
         <v>82</v>
       </c>
       <c r="B5" s="43" t="s">
@@ -4322,7 +4363,7 @@
         <v>145</v>
       </c>
       <c r="E5" s="53"/>
-      <c r="F5" s="92">
+      <c r="F5" s="67">
         <f t="shared" si="0"/>
         <v>0.44444444444444442</v>
       </c>
@@ -4341,7 +4382,7 @@
         <v>145</v>
       </c>
       <c r="E6" s="53"/>
-      <c r="F6" s="92">
+      <c r="F6" s="67">
         <f t="shared" si="0"/>
         <v>0.88888888888888884</v>
       </c>
@@ -4350,9 +4391,9 @@
       <c r="A7" s="44" t="s">
         <v>267</v>
       </c>
-      <c r="B7" s="81"/>
-      <c r="C7" s="82"/>
-      <c r="D7" s="83"/>
+      <c r="B7" s="75"/>
+      <c r="C7" s="76"/>
+      <c r="D7" s="77"/>
       <c r="E7" s="53"/>
     </row>
     <row r="8" spans="1:7">
@@ -4369,7 +4410,7 @@
         <v>18</v>
       </c>
       <c r="E8" s="53"/>
-      <c r="F8" s="92">
+      <c r="F8" s="67">
         <f>SUM((IF(B8="Sí",3,IF(B8="Regular",2,IF(B8="Parcialmente",2)))),(IF(C8="Sí",3,IF(C8="Regular",2,IF(C8="Parcialmente",2)))),(IF(D8="Sí",3,IF(D8="Regular",2,IF(D8="Parcialmente",2)))))/9</f>
         <v>0.66666666666666663</v>
       </c>
@@ -4392,7 +4433,7 @@
         <v>292</v>
       </c>
       <c r="E9" s="53"/>
-      <c r="F9" s="92">
+      <c r="F9" s="67">
         <f t="shared" ref="F9:F18" si="1">SUM((IF(B9="Sí",3,IF(B9="Regular",2,IF(B9="Parcialmente",2)))),(IF(C9="Sí",3,IF(C9="Regular",2,IF(C9="Parcialmente",2)))),(IF(D9="Sí",3,IF(D9="Regular",2,IF(D9="Parcialmente",2)))))/9</f>
         <v>0.77777777777777779</v>
       </c>
@@ -4411,13 +4452,13 @@
         <v>18</v>
       </c>
       <c r="E10" s="53"/>
-      <c r="F10" s="92">
+      <c r="F10" s="67">
         <f t="shared" si="1"/>
         <v>0.88888888888888884</v>
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="72" t="s">
+      <c r="A11" s="55" t="s">
         <v>87</v>
       </c>
       <c r="B11" s="43" t="s">
@@ -4430,7 +4471,7 @@
         <v>18</v>
       </c>
       <c r="E11" s="53"/>
-      <c r="F11" s="92">
+      <c r="F11" s="67">
         <f t="shared" si="1"/>
         <v>0.22222222222222221</v>
       </c>
@@ -4449,7 +4490,7 @@
         <v>293</v>
       </c>
       <c r="E12" s="53"/>
-      <c r="F12" s="92">
+      <c r="F12" s="67">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4458,9 +4499,9 @@
       <c r="A13" s="44" t="s">
         <v>88</v>
       </c>
-      <c r="B13" s="81"/>
-      <c r="C13" s="82"/>
-      <c r="D13" s="83"/>
+      <c r="B13" s="75"/>
+      <c r="C13" s="76"/>
+      <c r="D13" s="77"/>
       <c r="E13" s="53"/>
     </row>
     <row r="14" spans="1:7">
@@ -4477,7 +4518,7 @@
         <v>292</v>
       </c>
       <c r="E14" s="53"/>
-      <c r="F14" s="92">
+      <c r="F14" s="67">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -4496,7 +4537,7 @@
         <v>18</v>
       </c>
       <c r="E15" s="53"/>
-      <c r="F15" s="92">
+      <c r="F15" s="67">
         <f t="shared" si="1"/>
         <v>0.44444444444444442</v>
       </c>
@@ -4505,9 +4546,9 @@
       <c r="A16" s="44" t="s">
         <v>91</v>
       </c>
-      <c r="B16" s="84"/>
-      <c r="C16" s="85"/>
-      <c r="D16" s="86"/>
+      <c r="B16" s="59"/>
+      <c r="C16" s="60"/>
+      <c r="D16" s="61"/>
       <c r="E16" s="53"/>
     </row>
     <row r="17" spans="1:6">
@@ -4523,7 +4564,7 @@
       <c r="D17" s="43" t="s">
         <v>293</v>
       </c>
-      <c r="F17" s="92">
+      <c r="F17" s="67">
         <f t="shared" si="1"/>
         <v>0.66666666666666663</v>
       </c>
@@ -4541,7 +4582,7 @@
       <c r="D18" s="43" t="s">
         <v>293</v>
       </c>
-      <c r="F18" s="92">
+      <c r="F18" s="67">
         <f t="shared" si="1"/>
         <v>0.55555555555555558</v>
       </c>
@@ -4576,21 +4617,21 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="30.5" style="48" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.33203125" style="74" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" style="74" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" style="92" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.33203125" style="57" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" style="57" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" style="67" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7" style="48" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="10.83203125" style="48"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="78" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="88"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="63"/>
     </row>
     <row r="2" spans="1:6" ht="13" thickBot="1">
       <c r="A2" s="49"/>
@@ -4603,16 +4644,16 @@
       <c r="D2" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="89"/>
+      <c r="E2" s="64"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="40" t="s">
         <v>95</v>
       </c>
-      <c r="B3" s="79"/>
-      <c r="C3" s="79"/>
-      <c r="D3" s="80"/>
-      <c r="E3" s="89"/>
+      <c r="B3" s="81"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="64"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="42" t="s">
@@ -4627,13 +4668,13 @@
       <c r="D4" s="43" t="s">
         <v>292</v>
       </c>
-      <c r="E4" s="90">
+      <c r="E4" s="65">
         <f>SUM((IF(B4="Sí",3,IF(B4="Regular",2))),(IF(C4="Sí",3,IF(C4="Regular",2))),(IF(D4="Sí",3,IF(D4="Regular",2))))/9</f>
         <v>0.88888888888888884</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="72" t="s">
+      <c r="A5" s="55" t="s">
         <v>97</v>
       </c>
       <c r="B5" s="43" t="s">
@@ -4645,7 +4686,7 @@
       <c r="D5" s="43" t="s">
         <v>145</v>
       </c>
-      <c r="E5" s="90">
+      <c r="E5" s="65">
         <f t="shared" ref="E5:E14" si="0">SUM((IF(B5="Sí",3,IF(B5="Regular",2))),(IF(C5="Sí",3,IF(C5="Regular",2))),(IF(D5="Sí",3,IF(D5="Regular",2))))/9</f>
         <v>0.88888888888888884</v>
       </c>
@@ -4663,7 +4704,7 @@
       <c r="D6" s="43" t="s">
         <v>145</v>
       </c>
-      <c r="E6" s="90">
+      <c r="E6" s="65">
         <f t="shared" si="0"/>
         <v>0.88888888888888884</v>
       </c>
@@ -4681,7 +4722,7 @@
       <c r="D7" s="43" t="s">
         <v>292</v>
       </c>
-      <c r="E7" s="90">
+      <c r="E7" s="65">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -4690,10 +4731,10 @@
       <c r="A8" s="44" t="s">
         <v>100</v>
       </c>
-      <c r="B8" s="81"/>
-      <c r="C8" s="82"/>
-      <c r="D8" s="83"/>
-      <c r="E8" s="90"/>
+      <c r="B8" s="75"/>
+      <c r="C8" s="76"/>
+      <c r="D8" s="77"/>
+      <c r="E8" s="65"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="42" t="s">
@@ -4708,7 +4749,7 @@
       <c r="D9" s="43" t="s">
         <v>292</v>
       </c>
-      <c r="E9" s="90">
+      <c r="E9" s="65">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -4726,7 +4767,7 @@
       <c r="D10" s="43" t="s">
         <v>292</v>
       </c>
-      <c r="E10" s="90">
+      <c r="E10" s="65">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -4744,8 +4785,8 @@
       <c r="D11" s="43" t="s">
         <v>271</v>
       </c>
-      <c r="E11" s="90"/>
-      <c r="F11" s="93" t="s">
+      <c r="E11" s="65"/>
+      <c r="F11" s="68" t="s">
         <v>272</v>
       </c>
     </row>
@@ -4762,7 +4803,7 @@
       <c r="D12" s="43" t="s">
         <v>292</v>
       </c>
-      <c r="E12" s="90">
+      <c r="E12" s="65">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -4771,10 +4812,10 @@
       <c r="A13" s="44" t="s">
         <v>105</v>
       </c>
-      <c r="B13" s="84"/>
-      <c r="C13" s="85"/>
-      <c r="D13" s="86"/>
-      <c r="E13" s="90"/>
+      <c r="B13" s="59"/>
+      <c r="C13" s="60"/>
+      <c r="D13" s="61"/>
+      <c r="E13" s="65"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="42" t="s">
@@ -4789,13 +4830,13 @@
       <c r="D14" s="43" t="s">
         <v>292</v>
       </c>
-      <c r="E14" s="90">
+      <c r="E14" s="65">
         <f t="shared" si="0"/>
         <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="D15" s="74" t="s">
+      <c r="D15" s="57" t="s">
         <v>273</v>
       </c>
     </row>
@@ -4821,7 +4862,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A4" activePane="bottomLeft" state="frozenSplit"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -4830,18 +4871,18 @@
     <col min="1" max="1" width="42" style="48" customWidth="1"/>
     <col min="2" max="4" width="10.83203125" style="48" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2" style="48" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="92"/>
+    <col min="6" max="6" width="10.83203125" style="67"/>
     <col min="7" max="7" width="11" style="48" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="10.83203125" style="48"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="78" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="77"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="80"/>
       <c r="E1" s="45"/>
     </row>
     <row r="2" spans="1:6" ht="13" thickBot="1">
@@ -4861,9 +4902,9 @@
       <c r="A3" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="B3" s="79"/>
-      <c r="C3" s="79"/>
-      <c r="D3" s="80"/>
+      <c r="B3" s="81"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="82"/>
       <c r="E3" s="51"/>
     </row>
     <row r="4" spans="1:6">
@@ -4880,13 +4921,13 @@
         <v>145</v>
       </c>
       <c r="E4" s="52"/>
-      <c r="F4" s="92">
+      <c r="F4" s="67">
         <f>SUM((IF(B4="Sí",3,IF(B4="Regular",2))),(IF(C4="Sí",3,IF(C4="Regular",2))),(IF(D4="Sí",3,IF(D4="Regular",2))))/9</f>
         <v>0.55555555555555558</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="24">
-      <c r="A5" s="72" t="s">
+      <c r="A5" s="55" t="s">
         <v>110</v>
       </c>
       <c r="B5" s="43" t="s">
@@ -4899,7 +4940,7 @@
         <v>293</v>
       </c>
       <c r="E5" s="53"/>
-      <c r="F5" s="92">
+      <c r="F5" s="67">
         <f t="shared" ref="F5:F9" si="0">SUM((IF(B5="Sí",3,IF(B5="Regular",2))),(IF(C5="Sí",3,IF(C5="Regular",2))),(IF(D5="Sí",3,IF(D5="Regular",2))))/9</f>
         <v>0</v>
       </c>
@@ -4918,7 +4959,7 @@
         <v>145</v>
       </c>
       <c r="E6" s="53"/>
-      <c r="F6" s="92">
+      <c r="F6" s="67">
         <f>SUM((IF(B6="Sí",3,IF(B6="Regular",2,IF(B6="Bien",3)))),(IF(C6="Sí",3,IF(C6="Regular",2,IF(C6="Bien",3)))),(IF(D6="Sí",3,IF(D6="Regular",2,IF(D6="Bien",3)))))/9</f>
         <v>0.88888888888888884</v>
       </c>
@@ -4937,7 +4978,7 @@
         <v>292</v>
       </c>
       <c r="E7" s="53"/>
-      <c r="F7" s="92">
+      <c r="F7" s="67">
         <f t="shared" si="0"/>
         <v>0.66666666666666663</v>
       </c>
@@ -4956,7 +4997,7 @@
         <v>292</v>
       </c>
       <c r="E8" s="53"/>
-      <c r="F8" s="92">
+      <c r="F8" s="67">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -4975,13 +5016,13 @@
         <v>292</v>
       </c>
       <c r="E9" s="53"/>
-      <c r="F9" s="92">
+      <c r="F9" s="67">
         <f t="shared" si="0"/>
         <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="24">
-      <c r="A10" s="72" t="s">
+      <c r="A10" s="55" t="s">
         <v>304</v>
       </c>
       <c r="B10" s="43" t="s">
@@ -4994,39 +5035,39 @@
         <v>18</v>
       </c>
       <c r="E10" s="53"/>
-      <c r="F10" s="92">
+      <c r="F10" s="67">
         <f>SUM((IF(B10="Sí",3,IF(B10="Regular",2,IF(B10="Parcialmente",2)))),(IF(C10="Sí",3,IF(C10="Regular",2,IF(C10="Parcialmente",2)))),(IF(D10="Sí",3,IF(D10="Regular",2,IF(D10="Parcialmente",2)))))/9</f>
         <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="24" hidden="1">
-      <c r="A11" s="72" t="s">
+      <c r="A11" s="55" t="s">
         <v>302</v>
       </c>
       <c r="B11" s="43"/>
       <c r="C11" s="43"/>
       <c r="D11" s="43"/>
       <c r="E11" s="53"/>
-      <c r="F11" s="92">
+      <c r="F11" s="67">
         <f t="shared" ref="F11:F16" si="1">SUM((IF(B11="Sí",3,IF(B11="Regular",2,IF(B11="Parcialmente",2)))),(IF(C11="Sí",3,IF(C11="Regular",2,IF(C11="Parcialmente",2)))),(IF(D11="Sí",3,IF(D11="Regular",2,IF(D11="Parcialmente",2)))))/9</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="24" hidden="1">
-      <c r="A12" s="72" t="s">
+      <c r="A12" s="55" t="s">
         <v>303</v>
       </c>
       <c r="B12" s="43"/>
       <c r="C12" s="43"/>
       <c r="D12" s="43"/>
       <c r="E12" s="53"/>
-      <c r="F12" s="92">
+      <c r="F12" s="67">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="24">
-      <c r="A13" s="72" t="s">
+      <c r="A13" s="55" t="s">
         <v>305</v>
       </c>
       <c r="B13" s="43" t="s">
@@ -5039,13 +5080,13 @@
         <v>292</v>
       </c>
       <c r="E13" s="53"/>
-      <c r="F13" s="92">
+      <c r="F13" s="67">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="24">
-      <c r="A14" s="72" t="s">
+      <c r="A14" s="55" t="s">
         <v>112</v>
       </c>
       <c r="B14" s="43" t="s">
@@ -5058,13 +5099,13 @@
         <v>18</v>
       </c>
       <c r="E14" s="53"/>
-      <c r="F14" s="92">
+      <c r="F14" s="67">
         <f t="shared" si="1"/>
         <v>0.55555555555555558</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="72" t="s">
+      <c r="A15" s="55" t="s">
         <v>113</v>
       </c>
       <c r="B15" s="43" t="s">
@@ -5077,13 +5118,13 @@
         <v>146</v>
       </c>
       <c r="E15" s="53"/>
-      <c r="F15" s="92">
+      <c r="F15" s="67">
         <f>SUM((IF(B15="Sí",3,IF(B15="Regular",2,IF(B15="Bien",3)))),(IF(C15="Sí",3,IF(C15="Regular",2,IF(C15="Bien",3)))),(IF(D15="Sí",3,IF(D15="Regular",2,IF(D15="Bien",3)))))/9</f>
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="72" t="s">
+      <c r="A16" s="55" t="s">
         <v>114</v>
       </c>
       <c r="B16" s="43" t="s">
@@ -5096,7 +5137,7 @@
         <v>293</v>
       </c>
       <c r="E16" s="53"/>
-      <c r="F16" s="92">
+      <c r="F16" s="67">
         <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
@@ -5121,7 +5162,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
@@ -5133,12 +5174,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="83" t="s">
         <v>115</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="66"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="85"/>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:8" ht="16" thickBot="1">
@@ -5158,9 +5199,9 @@
       <c r="A3" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="B3" s="67"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="68"/>
+      <c r="B3" s="86"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="87"/>
       <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:8">
@@ -5260,9 +5301,9 @@
       <c r="A9" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="B9" s="61"/>
-      <c r="C9" s="62"/>
-      <c r="D9" s="63"/>
+      <c r="B9" s="88"/>
+      <c r="C9" s="89"/>
+      <c r="D9" s="90"/>
       <c r="E9" s="8"/>
     </row>
     <row r="10" spans="1:8" ht="45">
@@ -5510,7 +5551,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView topLeftCell="A21" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
@@ -5524,12 +5565,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18" customHeight="1">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="83" t="s">
         <v>130</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="66"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="85"/>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:8" ht="16" thickBot="1">
@@ -5549,9 +5590,9 @@
       <c r="A3" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="B3" s="67"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="68"/>
+      <c r="B3" s="86"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="87"/>
       <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:8" ht="30">
@@ -5573,9 +5614,9 @@
       <c r="A5" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="B5" s="61"/>
-      <c r="C5" s="62"/>
-      <c r="D5" s="63"/>
+      <c r="B5" s="88"/>
+      <c r="C5" s="89"/>
+      <c r="D5" s="90"/>
       <c r="E5" s="8"/>
     </row>
     <row r="6" spans="1:8">
@@ -5600,9 +5641,9 @@
       <c r="A7" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="B7" s="61"/>
-      <c r="C7" s="62"/>
-      <c r="D7" s="63"/>
+      <c r="B7" s="88"/>
+      <c r="C7" s="89"/>
+      <c r="D7" s="90"/>
       <c r="E7" s="8"/>
     </row>
     <row r="8" spans="1:8">
@@ -5648,9 +5689,9 @@
       <c r="A10" s="21" t="s">
         <v>143</v>
       </c>
-      <c r="B10" s="69"/>
-      <c r="C10" s="70"/>
-      <c r="D10" s="71"/>
+      <c r="B10" s="91"/>
+      <c r="C10" s="92"/>
+      <c r="D10" s="93"/>
       <c r="E10" s="8"/>
       <c r="F10" s="26"/>
       <c r="G10" s="26"/>
@@ -5702,9 +5743,9 @@
       <c r="A13" s="22" t="s">
         <v>148</v>
       </c>
-      <c r="B13" s="69"/>
-      <c r="C13" s="70"/>
-      <c r="D13" s="71"/>
+      <c r="B13" s="91"/>
+      <c r="C13" s="92"/>
+      <c r="D13" s="93"/>
       <c r="E13" s="8"/>
       <c r="F13" s="26"/>
       <c r="G13" s="26"/>
@@ -5738,9 +5779,9 @@
       <c r="A15" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="B15" s="61"/>
-      <c r="C15" s="62"/>
-      <c r="D15" s="63"/>
+      <c r="B15" s="88"/>
+      <c r="C15" s="89"/>
+      <c r="D15" s="90"/>
       <c r="E15" s="8"/>
     </row>
     <row r="16" spans="1:8">
@@ -5916,9 +5957,9 @@
       <c r="A24" s="16" t="s">
         <v>160</v>
       </c>
-      <c r="B24" s="61"/>
-      <c r="C24" s="62"/>
-      <c r="D24" s="63"/>
+      <c r="B24" s="88"/>
+      <c r="C24" s="89"/>
+      <c r="D24" s="90"/>
     </row>
     <row r="25" spans="1:9" ht="45">
       <c r="A25" s="4" t="s">
@@ -5972,7 +6013,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
@@ -5985,12 +6026,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="83" t="s">
         <v>162</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="66"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="85"/>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:7" ht="16" thickBot="1">
@@ -6010,9 +6051,9 @@
       <c r="A3" s="14" t="s">
         <v>183</v>
       </c>
-      <c r="B3" s="67"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="68"/>
+      <c r="B3" s="86"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="87"/>
       <c r="E3" s="6"/>
       <c r="F3" s="27" t="s">
         <v>173</v>
@@ -6357,9 +6398,9 @@
       <c r="A20" s="13" t="s">
         <v>190</v>
       </c>
-      <c r="B20" s="61"/>
-      <c r="C20" s="62"/>
-      <c r="D20" s="63"/>
+      <c r="B20" s="88"/>
+      <c r="C20" s="89"/>
+      <c r="D20" s="90"/>
       <c r="E20" s="8"/>
       <c r="F20" s="27" t="s">
         <v>175</v>
@@ -6513,9 +6554,9 @@
       <c r="A28" s="13" t="s">
         <v>191</v>
       </c>
-      <c r="B28" s="61"/>
-      <c r="C28" s="62"/>
-      <c r="D28" s="63"/>
+      <c r="B28" s="88"/>
+      <c r="C28" s="89"/>
+      <c r="D28" s="90"/>
       <c r="E28" s="8"/>
       <c r="F28" s="31"/>
       <c r="G28" s="31"/>
@@ -6592,7 +6633,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="B18" sqref="B18:D19"/>
     </sheetView>
   </sheetViews>
@@ -6604,12 +6645,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="83" t="s">
         <v>198</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="66"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="85"/>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5" ht="16" thickBot="1">
@@ -6629,9 +6670,9 @@
       <c r="A3" s="14" t="s">
         <v>199</v>
       </c>
-      <c r="B3" s="67"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="68"/>
+      <c r="B3" s="86"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="87"/>
       <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:5">
@@ -6683,9 +6724,9 @@
       <c r="A7" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="B7" s="61"/>
-      <c r="C7" s="62"/>
-      <c r="D7" s="63"/>
+      <c r="B7" s="88"/>
+      <c r="C7" s="89"/>
+      <c r="D7" s="90"/>
       <c r="E7" s="8"/>
     </row>
     <row r="8" spans="1:5">
@@ -6767,9 +6808,9 @@
       <c r="A13" s="13" t="s">
         <v>209</v>
       </c>
-      <c r="B13" s="61"/>
-      <c r="C13" s="62"/>
-      <c r="D13" s="63"/>
+      <c r="B13" s="88"/>
+      <c r="C13" s="89"/>
+      <c r="D13" s="90"/>
       <c r="E13" s="8"/>
     </row>
     <row r="14" spans="1:5">
@@ -6791,9 +6832,9 @@
       <c r="A15" s="13" t="s">
         <v>211</v>
       </c>
-      <c r="B15" s="61"/>
-      <c r="C15" s="62"/>
-      <c r="D15" s="63"/>
+      <c r="B15" s="88"/>
+      <c r="C15" s="89"/>
+      <c r="D15" s="90"/>
       <c r="E15" s="8"/>
     </row>
     <row r="16" spans="1:5" ht="30">
@@ -6815,9 +6856,9 @@
       <c r="A17" s="13" t="s">
         <v>213</v>
       </c>
-      <c r="B17" s="61"/>
-      <c r="C17" s="62"/>
-      <c r="D17" s="63"/>
+      <c r="B17" s="88"/>
+      <c r="C17" s="89"/>
+      <c r="D17" s="90"/>
       <c r="E17" s="8"/>
     </row>
     <row r="18" spans="1:5" ht="30">

</xml_diff>